<commit_message>
Cambios en datos ambientales
Ya están disponibles los datos actualizados de calidad de agua de la CEA Jalisco, por lo que adapté el código para que fuera compatible con esos datos crudos.
</commit_message>
<xml_diff>
--- a/datos/crudos/Cajititlán_Bio.xlsx
+++ b/datos/crudos/Cajititlán_Bio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccopi\Desktop\PP\Caji\datos\crudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE2142B-D8FA-4993-9A4F-8BF7D3DF61B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6B9D36-24FE-442E-8119-3E6284E212F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{23288B8C-CFF6-477E-BC6E-3C842449D796}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="800">
   <si>
     <t>Estación</t>
   </si>
@@ -2419,10 +2419,25 @@
     <t>est</t>
   </si>
   <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>month</t>
+    <t>LC-01</t>
+  </si>
+  <si>
+    <t>LC-02</t>
+  </si>
+  <si>
+    <t>LC-03</t>
+  </si>
+  <si>
+    <t>LC-04</t>
+  </si>
+  <si>
+    <t>LC-05</t>
+  </si>
+  <si>
+    <t>año</t>
+  </si>
+  <si>
+    <t>mes</t>
   </si>
 </sst>
 </file>
@@ -3095,8 +3110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F1F480-4040-4F5F-AC98-1E4CE20790A9}">
   <dimension ref="A1:LD65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26613,15 +26628,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD579EC3-DFCC-45CB-8CDA-ACC6EEAB4522}">
   <dimension ref="A1:LG68"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView topLeftCell="A52" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67:F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="11" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="16" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="21" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
@@ -44642,7 +44658,7 @@
     </row>
     <row r="65" spans="1:316" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>793</v>
+        <v>798</v>
       </c>
       <c r="B65">
         <v>2014</v>
@@ -45592,7 +45608,7 @@
     </row>
     <row r="66" spans="1:316" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>794</v>
+        <v>799</v>
       </c>
       <c r="B66">
         <v>10</v>
@@ -46544,950 +46560,950 @@
       <c r="A67" t="s">
         <v>792</v>
       </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67">
-        <v>2</v>
-      </c>
-      <c r="D67">
-        <v>3</v>
-      </c>
-      <c r="E67">
-        <v>4</v>
-      </c>
-      <c r="F67">
-        <v>5</v>
-      </c>
-      <c r="G67">
-        <v>1</v>
-      </c>
-      <c r="H67">
-        <v>2</v>
-      </c>
-      <c r="I67">
-        <v>3</v>
-      </c>
-      <c r="J67">
-        <v>4</v>
-      </c>
-      <c r="K67">
-        <v>5</v>
-      </c>
-      <c r="L67">
-        <v>1</v>
-      </c>
-      <c r="M67">
-        <v>2</v>
-      </c>
-      <c r="N67">
-        <v>3</v>
-      </c>
-      <c r="O67">
-        <v>4</v>
-      </c>
-      <c r="P67">
-        <v>5</v>
-      </c>
-      <c r="Q67">
-        <v>1</v>
-      </c>
-      <c r="R67">
-        <v>2</v>
-      </c>
-      <c r="S67">
-        <v>3</v>
-      </c>
-      <c r="T67">
-        <v>4</v>
-      </c>
-      <c r="U67">
-        <v>5</v>
-      </c>
-      <c r="V67">
-        <v>1</v>
-      </c>
-      <c r="W67">
-        <v>2</v>
-      </c>
-      <c r="X67">
-        <v>3</v>
-      </c>
-      <c r="Y67">
-        <v>4</v>
-      </c>
-      <c r="Z67">
-        <v>5</v>
-      </c>
-      <c r="AA67">
-        <v>1</v>
-      </c>
-      <c r="AB67">
-        <v>2</v>
-      </c>
-      <c r="AC67">
-        <v>3</v>
-      </c>
-      <c r="AD67">
-        <v>4</v>
-      </c>
-      <c r="AE67">
-        <v>5</v>
-      </c>
-      <c r="AF67">
-        <v>1</v>
-      </c>
-      <c r="AG67">
-        <v>2</v>
-      </c>
-      <c r="AH67">
-        <v>3</v>
-      </c>
-      <c r="AI67">
-        <v>4</v>
-      </c>
-      <c r="AJ67">
-        <v>5</v>
-      </c>
-      <c r="AK67">
-        <v>1</v>
-      </c>
-      <c r="AL67">
-        <v>2</v>
-      </c>
-      <c r="AM67">
-        <v>3</v>
-      </c>
-      <c r="AN67">
-        <v>4</v>
-      </c>
-      <c r="AO67">
-        <v>5</v>
-      </c>
-      <c r="AP67">
-        <v>1</v>
-      </c>
-      <c r="AQ67">
-        <v>2</v>
-      </c>
-      <c r="AR67">
-        <v>3</v>
-      </c>
-      <c r="AS67">
-        <v>4</v>
-      </c>
-      <c r="AT67">
-        <v>5</v>
-      </c>
-      <c r="AU67">
-        <v>1</v>
-      </c>
-      <c r="AV67">
-        <v>2</v>
-      </c>
-      <c r="AW67">
-        <v>3</v>
-      </c>
-      <c r="AX67">
-        <v>4</v>
-      </c>
-      <c r="AY67">
-        <v>5</v>
-      </c>
-      <c r="AZ67">
-        <v>1</v>
-      </c>
-      <c r="BA67">
-        <v>2</v>
-      </c>
-      <c r="BB67">
-        <v>3</v>
-      </c>
-      <c r="BC67">
-        <v>4</v>
-      </c>
-      <c r="BD67">
-        <v>5</v>
-      </c>
-      <c r="BE67">
-        <v>1</v>
-      </c>
-      <c r="BF67">
-        <v>2</v>
-      </c>
-      <c r="BG67">
-        <v>3</v>
-      </c>
-      <c r="BH67">
-        <v>4</v>
-      </c>
-      <c r="BI67">
-        <v>5</v>
-      </c>
-      <c r="BJ67">
-        <v>1</v>
-      </c>
-      <c r="BK67">
-        <v>2</v>
-      </c>
-      <c r="BL67">
-        <v>3</v>
-      </c>
-      <c r="BM67">
-        <v>4</v>
-      </c>
-      <c r="BN67">
-        <v>5</v>
-      </c>
-      <c r="BO67">
-        <v>1</v>
-      </c>
-      <c r="BP67">
-        <v>2</v>
-      </c>
-      <c r="BQ67">
-        <v>3</v>
-      </c>
-      <c r="BR67">
-        <v>4</v>
-      </c>
-      <c r="BS67">
-        <v>5</v>
-      </c>
-      <c r="BT67">
-        <v>1</v>
-      </c>
-      <c r="BU67">
-        <v>2</v>
-      </c>
-      <c r="BV67">
-        <v>3</v>
-      </c>
-      <c r="BW67">
-        <v>4</v>
-      </c>
-      <c r="BX67">
-        <v>5</v>
-      </c>
-      <c r="BY67">
-        <v>1</v>
-      </c>
-      <c r="BZ67">
-        <v>2</v>
-      </c>
-      <c r="CA67">
-        <v>3</v>
-      </c>
-      <c r="CB67">
-        <v>4</v>
-      </c>
-      <c r="CC67">
-        <v>5</v>
-      </c>
-      <c r="CD67">
-        <v>1</v>
-      </c>
-      <c r="CE67">
-        <v>2</v>
-      </c>
-      <c r="CF67">
-        <v>3</v>
-      </c>
-      <c r="CG67">
-        <v>4</v>
-      </c>
-      <c r="CH67">
-        <v>5</v>
-      </c>
-      <c r="CI67">
-        <v>1</v>
-      </c>
-      <c r="CJ67">
-        <v>2</v>
-      </c>
-      <c r="CK67">
-        <v>3</v>
-      </c>
-      <c r="CL67">
-        <v>4</v>
-      </c>
-      <c r="CM67">
-        <v>5</v>
-      </c>
-      <c r="CN67">
-        <v>1</v>
-      </c>
-      <c r="CO67">
-        <v>2</v>
-      </c>
-      <c r="CP67">
-        <v>3</v>
-      </c>
-      <c r="CQ67">
-        <v>4</v>
-      </c>
-      <c r="CR67">
-        <v>5</v>
-      </c>
-      <c r="CS67">
-        <v>1</v>
-      </c>
-      <c r="CT67">
-        <v>2</v>
-      </c>
-      <c r="CU67">
-        <v>3</v>
-      </c>
-      <c r="CV67">
-        <v>4</v>
-      </c>
-      <c r="CW67">
-        <v>5</v>
-      </c>
-      <c r="CX67">
-        <v>1</v>
-      </c>
-      <c r="CY67">
-        <v>2</v>
-      </c>
-      <c r="CZ67">
-        <v>3</v>
-      </c>
-      <c r="DA67">
-        <v>4</v>
-      </c>
-      <c r="DB67">
-        <v>5</v>
-      </c>
-      <c r="DC67">
-        <v>1</v>
-      </c>
-      <c r="DD67">
-        <v>2</v>
-      </c>
-      <c r="DE67">
-        <v>3</v>
-      </c>
-      <c r="DF67">
-        <v>4</v>
-      </c>
-      <c r="DG67">
-        <v>5</v>
-      </c>
-      <c r="DH67">
-        <v>1</v>
-      </c>
-      <c r="DI67">
-        <v>2</v>
-      </c>
-      <c r="DJ67">
-        <v>3</v>
-      </c>
-      <c r="DK67">
-        <v>4</v>
-      </c>
-      <c r="DL67">
-        <v>5</v>
-      </c>
-      <c r="DM67">
-        <v>1</v>
-      </c>
-      <c r="DN67">
-        <v>2</v>
-      </c>
-      <c r="DO67">
-        <v>3</v>
-      </c>
-      <c r="DP67">
-        <v>4</v>
-      </c>
-      <c r="DQ67">
-        <v>5</v>
-      </c>
-      <c r="DR67">
-        <v>1</v>
-      </c>
-      <c r="DS67">
-        <v>2</v>
-      </c>
-      <c r="DT67">
-        <v>3</v>
-      </c>
-      <c r="DU67">
-        <v>4</v>
-      </c>
-      <c r="DV67">
-        <v>5</v>
-      </c>
-      <c r="DW67">
-        <v>1</v>
-      </c>
-      <c r="DX67">
-        <v>2</v>
-      </c>
-      <c r="DY67">
-        <v>3</v>
-      </c>
-      <c r="DZ67">
-        <v>4</v>
-      </c>
-      <c r="EA67">
-        <v>5</v>
-      </c>
-      <c r="EB67">
-        <v>1</v>
-      </c>
-      <c r="EC67">
-        <v>2</v>
-      </c>
-      <c r="ED67">
-        <v>3</v>
-      </c>
-      <c r="EE67">
-        <v>4</v>
-      </c>
-      <c r="EF67">
-        <v>5</v>
-      </c>
-      <c r="EG67">
-        <v>1</v>
-      </c>
-      <c r="EH67">
-        <v>2</v>
-      </c>
-      <c r="EI67">
-        <v>3</v>
-      </c>
-      <c r="EJ67">
-        <v>4</v>
-      </c>
-      <c r="EK67">
-        <v>5</v>
-      </c>
-      <c r="EL67">
-        <v>1</v>
-      </c>
-      <c r="EM67">
-        <v>2</v>
-      </c>
-      <c r="EN67">
-        <v>3</v>
-      </c>
-      <c r="EO67">
-        <v>4</v>
-      </c>
-      <c r="EP67">
-        <v>5</v>
-      </c>
-      <c r="EQ67">
-        <v>1</v>
-      </c>
-      <c r="ER67">
-        <v>2</v>
-      </c>
-      <c r="ES67">
-        <v>3</v>
-      </c>
-      <c r="ET67">
-        <v>4</v>
-      </c>
-      <c r="EU67">
-        <v>5</v>
-      </c>
-      <c r="EV67">
-        <v>1</v>
-      </c>
-      <c r="EW67">
-        <v>2</v>
-      </c>
-      <c r="EX67">
-        <v>3</v>
-      </c>
-      <c r="EY67">
-        <v>4</v>
-      </c>
-      <c r="EZ67">
-        <v>5</v>
-      </c>
-      <c r="FA67">
-        <v>1</v>
-      </c>
-      <c r="FB67">
-        <v>2</v>
-      </c>
-      <c r="FC67">
-        <v>3</v>
-      </c>
-      <c r="FD67">
-        <v>4</v>
-      </c>
-      <c r="FE67">
-        <v>5</v>
-      </c>
-      <c r="FF67">
-        <v>1</v>
-      </c>
-      <c r="FG67">
-        <v>2</v>
-      </c>
-      <c r="FH67">
-        <v>3</v>
-      </c>
-      <c r="FI67">
-        <v>4</v>
-      </c>
-      <c r="FJ67">
-        <v>5</v>
-      </c>
-      <c r="FK67">
-        <v>1</v>
-      </c>
-      <c r="FL67">
-        <v>2</v>
-      </c>
-      <c r="FM67">
-        <v>3</v>
-      </c>
-      <c r="FN67">
-        <v>4</v>
-      </c>
-      <c r="FO67">
-        <v>5</v>
-      </c>
-      <c r="FP67">
-        <v>1</v>
-      </c>
-      <c r="FQ67">
-        <v>2</v>
-      </c>
-      <c r="FR67">
-        <v>3</v>
-      </c>
-      <c r="FS67">
-        <v>4</v>
-      </c>
-      <c r="FT67">
-        <v>5</v>
-      </c>
-      <c r="FU67">
-        <v>1</v>
-      </c>
-      <c r="FV67">
-        <v>2</v>
-      </c>
-      <c r="FW67">
-        <v>3</v>
-      </c>
-      <c r="FX67">
-        <v>4</v>
-      </c>
-      <c r="FY67">
-        <v>5</v>
-      </c>
-      <c r="FZ67">
-        <v>1</v>
-      </c>
-      <c r="GA67">
-        <v>2</v>
-      </c>
-      <c r="GB67">
-        <v>3</v>
-      </c>
-      <c r="GC67">
-        <v>4</v>
-      </c>
-      <c r="GD67">
-        <v>5</v>
-      </c>
-      <c r="GE67">
-        <v>1</v>
-      </c>
-      <c r="GF67">
-        <v>2</v>
-      </c>
-      <c r="GG67">
-        <v>3</v>
-      </c>
-      <c r="GH67">
-        <v>4</v>
-      </c>
-      <c r="GI67">
-        <v>5</v>
-      </c>
-      <c r="GJ67">
-        <v>1</v>
-      </c>
-      <c r="GK67">
-        <v>2</v>
-      </c>
-      <c r="GL67">
-        <v>3</v>
-      </c>
-      <c r="GM67">
-        <v>4</v>
-      </c>
-      <c r="GN67">
-        <v>5</v>
-      </c>
-      <c r="GO67">
-        <v>1</v>
-      </c>
-      <c r="GP67">
-        <v>2</v>
-      </c>
-      <c r="GQ67">
-        <v>3</v>
-      </c>
-      <c r="GR67">
-        <v>4</v>
-      </c>
-      <c r="GS67">
-        <v>5</v>
-      </c>
-      <c r="GT67">
-        <v>1</v>
-      </c>
-      <c r="GU67">
-        <v>2</v>
-      </c>
-      <c r="GV67">
-        <v>3</v>
-      </c>
-      <c r="GW67">
-        <v>4</v>
-      </c>
-      <c r="GX67">
-        <v>5</v>
-      </c>
-      <c r="GY67">
-        <v>1</v>
-      </c>
-      <c r="GZ67">
-        <v>2</v>
-      </c>
-      <c r="HA67">
-        <v>3</v>
-      </c>
-      <c r="HB67">
-        <v>4</v>
-      </c>
-      <c r="HC67">
-        <v>5</v>
-      </c>
-      <c r="HD67">
-        <v>1</v>
-      </c>
-      <c r="HE67">
-        <v>2</v>
-      </c>
-      <c r="HF67">
-        <v>3</v>
-      </c>
-      <c r="HG67">
-        <v>4</v>
-      </c>
-      <c r="HH67">
-        <v>5</v>
-      </c>
-      <c r="HI67">
-        <v>1</v>
-      </c>
-      <c r="HJ67">
-        <v>2</v>
-      </c>
-      <c r="HK67">
-        <v>3</v>
-      </c>
-      <c r="HL67">
-        <v>4</v>
-      </c>
-      <c r="HM67">
-        <v>5</v>
-      </c>
-      <c r="HN67">
-        <v>1</v>
-      </c>
-      <c r="HO67">
-        <v>2</v>
-      </c>
-      <c r="HP67">
-        <v>3</v>
-      </c>
-      <c r="HQ67">
-        <v>4</v>
-      </c>
-      <c r="HR67">
-        <v>5</v>
-      </c>
-      <c r="HS67">
-        <v>1</v>
-      </c>
-      <c r="HT67">
-        <v>2</v>
-      </c>
-      <c r="HU67">
-        <v>3</v>
-      </c>
-      <c r="HV67">
-        <v>4</v>
-      </c>
-      <c r="HW67">
-        <v>5</v>
-      </c>
-      <c r="HX67">
-        <v>1</v>
-      </c>
-      <c r="HY67">
-        <v>2</v>
-      </c>
-      <c r="HZ67">
-        <v>3</v>
-      </c>
-      <c r="IA67">
-        <v>4</v>
-      </c>
-      <c r="IB67">
-        <v>5</v>
-      </c>
-      <c r="IC67">
-        <v>1</v>
-      </c>
-      <c r="ID67">
-        <v>2</v>
-      </c>
-      <c r="IE67">
-        <v>3</v>
-      </c>
-      <c r="IF67">
-        <v>4</v>
-      </c>
-      <c r="IG67">
-        <v>5</v>
-      </c>
-      <c r="IH67">
-        <v>1</v>
-      </c>
-      <c r="II67">
-        <v>2</v>
-      </c>
-      <c r="IJ67">
-        <v>3</v>
-      </c>
-      <c r="IK67">
-        <v>4</v>
-      </c>
-      <c r="IL67">
-        <v>5</v>
-      </c>
-      <c r="IM67">
-        <v>1</v>
-      </c>
-      <c r="IN67">
-        <v>2</v>
-      </c>
-      <c r="IO67">
-        <v>3</v>
-      </c>
-      <c r="IP67">
-        <v>4</v>
-      </c>
-      <c r="IQ67">
-        <v>5</v>
-      </c>
-      <c r="IR67">
-        <v>1</v>
-      </c>
-      <c r="IS67">
-        <v>2</v>
-      </c>
-      <c r="IT67">
-        <v>3</v>
-      </c>
-      <c r="IU67">
-        <v>4</v>
-      </c>
-      <c r="IV67">
-        <v>5</v>
-      </c>
-      <c r="IW67">
-        <v>1</v>
-      </c>
-      <c r="IX67">
-        <v>2</v>
-      </c>
-      <c r="IY67">
-        <v>3</v>
-      </c>
-      <c r="IZ67">
-        <v>4</v>
-      </c>
-      <c r="JA67">
-        <v>5</v>
-      </c>
-      <c r="JB67">
-        <v>1</v>
-      </c>
-      <c r="JC67">
-        <v>2</v>
-      </c>
-      <c r="JD67">
-        <v>3</v>
-      </c>
-      <c r="JE67">
-        <v>4</v>
-      </c>
-      <c r="JF67">
-        <v>5</v>
-      </c>
-      <c r="JG67">
-        <v>1</v>
-      </c>
-      <c r="JH67">
-        <v>2</v>
-      </c>
-      <c r="JI67">
-        <v>3</v>
-      </c>
-      <c r="JJ67">
-        <v>4</v>
-      </c>
-      <c r="JK67">
-        <v>5</v>
-      </c>
-      <c r="JL67">
-        <v>1</v>
-      </c>
-      <c r="JM67">
-        <v>2</v>
-      </c>
-      <c r="JN67">
-        <v>3</v>
-      </c>
-      <c r="JO67">
-        <v>4</v>
-      </c>
-      <c r="JP67">
-        <v>5</v>
-      </c>
-      <c r="JQ67">
-        <v>1</v>
-      </c>
-      <c r="JR67">
-        <v>2</v>
-      </c>
-      <c r="JS67">
-        <v>3</v>
-      </c>
-      <c r="JT67">
-        <v>4</v>
-      </c>
-      <c r="JU67">
-        <v>5</v>
-      </c>
-      <c r="JV67">
-        <v>1</v>
-      </c>
-      <c r="JW67">
-        <v>2</v>
-      </c>
-      <c r="JX67">
-        <v>3</v>
-      </c>
-      <c r="JY67">
-        <v>4</v>
-      </c>
-      <c r="JZ67">
-        <v>5</v>
-      </c>
-      <c r="KA67">
-        <v>1</v>
-      </c>
-      <c r="KB67">
-        <v>2</v>
-      </c>
-      <c r="KC67">
-        <v>3</v>
-      </c>
-      <c r="KD67">
-        <v>4</v>
-      </c>
-      <c r="KE67">
-        <v>5</v>
-      </c>
-      <c r="KF67">
-        <v>1</v>
-      </c>
-      <c r="KG67">
-        <v>2</v>
-      </c>
-      <c r="KH67">
-        <v>3</v>
-      </c>
-      <c r="KI67">
-        <v>4</v>
-      </c>
-      <c r="KJ67">
-        <v>5</v>
-      </c>
-      <c r="KK67">
-        <v>1</v>
-      </c>
-      <c r="KL67">
-        <v>2</v>
-      </c>
-      <c r="KM67">
-        <v>3</v>
-      </c>
-      <c r="KN67">
-        <v>4</v>
-      </c>
-      <c r="KO67">
-        <v>5</v>
-      </c>
-      <c r="KP67">
-        <v>1</v>
-      </c>
-      <c r="KQ67">
-        <v>2</v>
-      </c>
-      <c r="KR67">
-        <v>3</v>
-      </c>
-      <c r="KS67">
-        <v>4</v>
-      </c>
-      <c r="KT67">
-        <v>5</v>
-      </c>
-      <c r="KU67">
-        <v>1</v>
-      </c>
-      <c r="KV67">
-        <v>2</v>
-      </c>
-      <c r="KW67">
-        <v>3</v>
-      </c>
-      <c r="KX67">
-        <v>4</v>
-      </c>
-      <c r="KY67">
-        <v>5</v>
-      </c>
-      <c r="KZ67">
-        <v>1</v>
-      </c>
-      <c r="LA67">
-        <v>2</v>
-      </c>
-      <c r="LB67">
-        <v>3</v>
-      </c>
-      <c r="LC67">
-        <v>4</v>
-      </c>
-      <c r="LD67">
-        <v>5</v>
+      <c r="B67" t="s">
+        <v>793</v>
+      </c>
+      <c r="C67" t="s">
+        <v>794</v>
+      </c>
+      <c r="D67" t="s">
+        <v>795</v>
+      </c>
+      <c r="E67" t="s">
+        <v>796</v>
+      </c>
+      <c r="F67" t="s">
+        <v>797</v>
+      </c>
+      <c r="G67" t="s">
+        <v>793</v>
+      </c>
+      <c r="H67" t="s">
+        <v>794</v>
+      </c>
+      <c r="I67" t="s">
+        <v>795</v>
+      </c>
+      <c r="J67" t="s">
+        <v>796</v>
+      </c>
+      <c r="K67" t="s">
+        <v>797</v>
+      </c>
+      <c r="L67" t="s">
+        <v>793</v>
+      </c>
+      <c r="M67" t="s">
+        <v>794</v>
+      </c>
+      <c r="N67" t="s">
+        <v>795</v>
+      </c>
+      <c r="O67" t="s">
+        <v>796</v>
+      </c>
+      <c r="P67" t="s">
+        <v>797</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>793</v>
+      </c>
+      <c r="R67" t="s">
+        <v>794</v>
+      </c>
+      <c r="S67" t="s">
+        <v>795</v>
+      </c>
+      <c r="T67" t="s">
+        <v>796</v>
+      </c>
+      <c r="U67" t="s">
+        <v>797</v>
+      </c>
+      <c r="V67" t="s">
+        <v>793</v>
+      </c>
+      <c r="W67" t="s">
+        <v>794</v>
+      </c>
+      <c r="X67" t="s">
+        <v>795</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>796</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>797</v>
+      </c>
+      <c r="AA67" t="s">
+        <v>793</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>794</v>
+      </c>
+      <c r="AC67" t="s">
+        <v>795</v>
+      </c>
+      <c r="AD67" t="s">
+        <v>796</v>
+      </c>
+      <c r="AE67" t="s">
+        <v>797</v>
+      </c>
+      <c r="AF67" t="s">
+        <v>793</v>
+      </c>
+      <c r="AG67" t="s">
+        <v>794</v>
+      </c>
+      <c r="AH67" t="s">
+        <v>795</v>
+      </c>
+      <c r="AI67" t="s">
+        <v>796</v>
+      </c>
+      <c r="AJ67" t="s">
+        <v>797</v>
+      </c>
+      <c r="AK67" t="s">
+        <v>793</v>
+      </c>
+      <c r="AL67" t="s">
+        <v>794</v>
+      </c>
+      <c r="AM67" t="s">
+        <v>795</v>
+      </c>
+      <c r="AN67" t="s">
+        <v>796</v>
+      </c>
+      <c r="AO67" t="s">
+        <v>797</v>
+      </c>
+      <c r="AP67" t="s">
+        <v>793</v>
+      </c>
+      <c r="AQ67" t="s">
+        <v>794</v>
+      </c>
+      <c r="AR67" t="s">
+        <v>795</v>
+      </c>
+      <c r="AS67" t="s">
+        <v>796</v>
+      </c>
+      <c r="AT67" t="s">
+        <v>797</v>
+      </c>
+      <c r="AU67" t="s">
+        <v>793</v>
+      </c>
+      <c r="AV67" t="s">
+        <v>794</v>
+      </c>
+      <c r="AW67" t="s">
+        <v>795</v>
+      </c>
+      <c r="AX67" t="s">
+        <v>796</v>
+      </c>
+      <c r="AY67" t="s">
+        <v>797</v>
+      </c>
+      <c r="AZ67" t="s">
+        <v>793</v>
+      </c>
+      <c r="BA67" t="s">
+        <v>794</v>
+      </c>
+      <c r="BB67" t="s">
+        <v>795</v>
+      </c>
+      <c r="BC67" t="s">
+        <v>796</v>
+      </c>
+      <c r="BD67" t="s">
+        <v>797</v>
+      </c>
+      <c r="BE67" t="s">
+        <v>793</v>
+      </c>
+      <c r="BF67" t="s">
+        <v>794</v>
+      </c>
+      <c r="BG67" t="s">
+        <v>795</v>
+      </c>
+      <c r="BH67" t="s">
+        <v>796</v>
+      </c>
+      <c r="BI67" t="s">
+        <v>797</v>
+      </c>
+      <c r="BJ67" t="s">
+        <v>793</v>
+      </c>
+      <c r="BK67" t="s">
+        <v>794</v>
+      </c>
+      <c r="BL67" t="s">
+        <v>795</v>
+      </c>
+      <c r="BM67" t="s">
+        <v>796</v>
+      </c>
+      <c r="BN67" t="s">
+        <v>797</v>
+      </c>
+      <c r="BO67" t="s">
+        <v>793</v>
+      </c>
+      <c r="BP67" t="s">
+        <v>794</v>
+      </c>
+      <c r="BQ67" t="s">
+        <v>795</v>
+      </c>
+      <c r="BR67" t="s">
+        <v>796</v>
+      </c>
+      <c r="BS67" t="s">
+        <v>797</v>
+      </c>
+      <c r="BT67" t="s">
+        <v>793</v>
+      </c>
+      <c r="BU67" t="s">
+        <v>794</v>
+      </c>
+      <c r="BV67" t="s">
+        <v>795</v>
+      </c>
+      <c r="BW67" t="s">
+        <v>796</v>
+      </c>
+      <c r="BX67" t="s">
+        <v>797</v>
+      </c>
+      <c r="BY67" t="s">
+        <v>793</v>
+      </c>
+      <c r="BZ67" t="s">
+        <v>794</v>
+      </c>
+      <c r="CA67" t="s">
+        <v>795</v>
+      </c>
+      <c r="CB67" t="s">
+        <v>796</v>
+      </c>
+      <c r="CC67" t="s">
+        <v>797</v>
+      </c>
+      <c r="CD67" t="s">
+        <v>793</v>
+      </c>
+      <c r="CE67" t="s">
+        <v>794</v>
+      </c>
+      <c r="CF67" t="s">
+        <v>795</v>
+      </c>
+      <c r="CG67" t="s">
+        <v>796</v>
+      </c>
+      <c r="CH67" t="s">
+        <v>797</v>
+      </c>
+      <c r="CI67" t="s">
+        <v>793</v>
+      </c>
+      <c r="CJ67" t="s">
+        <v>794</v>
+      </c>
+      <c r="CK67" t="s">
+        <v>795</v>
+      </c>
+      <c r="CL67" t="s">
+        <v>796</v>
+      </c>
+      <c r="CM67" t="s">
+        <v>797</v>
+      </c>
+      <c r="CN67" t="s">
+        <v>793</v>
+      </c>
+      <c r="CO67" t="s">
+        <v>794</v>
+      </c>
+      <c r="CP67" t="s">
+        <v>795</v>
+      </c>
+      <c r="CQ67" t="s">
+        <v>796</v>
+      </c>
+      <c r="CR67" t="s">
+        <v>797</v>
+      </c>
+      <c r="CS67" t="s">
+        <v>793</v>
+      </c>
+      <c r="CT67" t="s">
+        <v>794</v>
+      </c>
+      <c r="CU67" t="s">
+        <v>795</v>
+      </c>
+      <c r="CV67" t="s">
+        <v>796</v>
+      </c>
+      <c r="CW67" t="s">
+        <v>797</v>
+      </c>
+      <c r="CX67" t="s">
+        <v>793</v>
+      </c>
+      <c r="CY67" t="s">
+        <v>794</v>
+      </c>
+      <c r="CZ67" t="s">
+        <v>795</v>
+      </c>
+      <c r="DA67" t="s">
+        <v>796</v>
+      </c>
+      <c r="DB67" t="s">
+        <v>797</v>
+      </c>
+      <c r="DC67" t="s">
+        <v>793</v>
+      </c>
+      <c r="DD67" t="s">
+        <v>794</v>
+      </c>
+      <c r="DE67" t="s">
+        <v>795</v>
+      </c>
+      <c r="DF67" t="s">
+        <v>796</v>
+      </c>
+      <c r="DG67" t="s">
+        <v>797</v>
+      </c>
+      <c r="DH67" t="s">
+        <v>793</v>
+      </c>
+      <c r="DI67" t="s">
+        <v>794</v>
+      </c>
+      <c r="DJ67" t="s">
+        <v>795</v>
+      </c>
+      <c r="DK67" t="s">
+        <v>796</v>
+      </c>
+      <c r="DL67" t="s">
+        <v>797</v>
+      </c>
+      <c r="DM67" t="s">
+        <v>793</v>
+      </c>
+      <c r="DN67" t="s">
+        <v>794</v>
+      </c>
+      <c r="DO67" t="s">
+        <v>795</v>
+      </c>
+      <c r="DP67" t="s">
+        <v>796</v>
+      </c>
+      <c r="DQ67" t="s">
+        <v>797</v>
+      </c>
+      <c r="DR67" t="s">
+        <v>793</v>
+      </c>
+      <c r="DS67" t="s">
+        <v>794</v>
+      </c>
+      <c r="DT67" t="s">
+        <v>795</v>
+      </c>
+      <c r="DU67" t="s">
+        <v>796</v>
+      </c>
+      <c r="DV67" t="s">
+        <v>797</v>
+      </c>
+      <c r="DW67" t="s">
+        <v>793</v>
+      </c>
+      <c r="DX67" t="s">
+        <v>794</v>
+      </c>
+      <c r="DY67" t="s">
+        <v>795</v>
+      </c>
+      <c r="DZ67" t="s">
+        <v>796</v>
+      </c>
+      <c r="EA67" t="s">
+        <v>797</v>
+      </c>
+      <c r="EB67" t="s">
+        <v>793</v>
+      </c>
+      <c r="EC67" t="s">
+        <v>794</v>
+      </c>
+      <c r="ED67" t="s">
+        <v>795</v>
+      </c>
+      <c r="EE67" t="s">
+        <v>796</v>
+      </c>
+      <c r="EF67" t="s">
+        <v>797</v>
+      </c>
+      <c r="EG67" t="s">
+        <v>793</v>
+      </c>
+      <c r="EH67" t="s">
+        <v>794</v>
+      </c>
+      <c r="EI67" t="s">
+        <v>795</v>
+      </c>
+      <c r="EJ67" t="s">
+        <v>796</v>
+      </c>
+      <c r="EK67" t="s">
+        <v>797</v>
+      </c>
+      <c r="EL67" t="s">
+        <v>793</v>
+      </c>
+      <c r="EM67" t="s">
+        <v>794</v>
+      </c>
+      <c r="EN67" t="s">
+        <v>795</v>
+      </c>
+      <c r="EO67" t="s">
+        <v>796</v>
+      </c>
+      <c r="EP67" t="s">
+        <v>797</v>
+      </c>
+      <c r="EQ67" t="s">
+        <v>793</v>
+      </c>
+      <c r="ER67" t="s">
+        <v>794</v>
+      </c>
+      <c r="ES67" t="s">
+        <v>795</v>
+      </c>
+      <c r="ET67" t="s">
+        <v>796</v>
+      </c>
+      <c r="EU67" t="s">
+        <v>797</v>
+      </c>
+      <c r="EV67" t="s">
+        <v>793</v>
+      </c>
+      <c r="EW67" t="s">
+        <v>794</v>
+      </c>
+      <c r="EX67" t="s">
+        <v>795</v>
+      </c>
+      <c r="EY67" t="s">
+        <v>796</v>
+      </c>
+      <c r="EZ67" t="s">
+        <v>797</v>
+      </c>
+      <c r="FA67" t="s">
+        <v>793</v>
+      </c>
+      <c r="FB67" t="s">
+        <v>794</v>
+      </c>
+      <c r="FC67" t="s">
+        <v>795</v>
+      </c>
+      <c r="FD67" t="s">
+        <v>796</v>
+      </c>
+      <c r="FE67" t="s">
+        <v>797</v>
+      </c>
+      <c r="FF67" t="s">
+        <v>793</v>
+      </c>
+      <c r="FG67" t="s">
+        <v>794</v>
+      </c>
+      <c r="FH67" t="s">
+        <v>795</v>
+      </c>
+      <c r="FI67" t="s">
+        <v>796</v>
+      </c>
+      <c r="FJ67" t="s">
+        <v>797</v>
+      </c>
+      <c r="FK67" t="s">
+        <v>793</v>
+      </c>
+      <c r="FL67" t="s">
+        <v>794</v>
+      </c>
+      <c r="FM67" t="s">
+        <v>795</v>
+      </c>
+      <c r="FN67" t="s">
+        <v>796</v>
+      </c>
+      <c r="FO67" t="s">
+        <v>797</v>
+      </c>
+      <c r="FP67" t="s">
+        <v>793</v>
+      </c>
+      <c r="FQ67" t="s">
+        <v>794</v>
+      </c>
+      <c r="FR67" t="s">
+        <v>795</v>
+      </c>
+      <c r="FS67" t="s">
+        <v>796</v>
+      </c>
+      <c r="FT67" t="s">
+        <v>797</v>
+      </c>
+      <c r="FU67" t="s">
+        <v>793</v>
+      </c>
+      <c r="FV67" t="s">
+        <v>794</v>
+      </c>
+      <c r="FW67" t="s">
+        <v>795</v>
+      </c>
+      <c r="FX67" t="s">
+        <v>796</v>
+      </c>
+      <c r="FY67" t="s">
+        <v>797</v>
+      </c>
+      <c r="FZ67" t="s">
+        <v>793</v>
+      </c>
+      <c r="GA67" t="s">
+        <v>794</v>
+      </c>
+      <c r="GB67" t="s">
+        <v>795</v>
+      </c>
+      <c r="GC67" t="s">
+        <v>796</v>
+      </c>
+      <c r="GD67" t="s">
+        <v>797</v>
+      </c>
+      <c r="GE67" t="s">
+        <v>793</v>
+      </c>
+      <c r="GF67" t="s">
+        <v>794</v>
+      </c>
+      <c r="GG67" t="s">
+        <v>795</v>
+      </c>
+      <c r="GH67" t="s">
+        <v>796</v>
+      </c>
+      <c r="GI67" t="s">
+        <v>797</v>
+      </c>
+      <c r="GJ67" t="s">
+        <v>793</v>
+      </c>
+      <c r="GK67" t="s">
+        <v>794</v>
+      </c>
+      <c r="GL67" t="s">
+        <v>795</v>
+      </c>
+      <c r="GM67" t="s">
+        <v>796</v>
+      </c>
+      <c r="GN67" t="s">
+        <v>797</v>
+      </c>
+      <c r="GO67" t="s">
+        <v>793</v>
+      </c>
+      <c r="GP67" t="s">
+        <v>794</v>
+      </c>
+      <c r="GQ67" t="s">
+        <v>795</v>
+      </c>
+      <c r="GR67" t="s">
+        <v>796</v>
+      </c>
+      <c r="GS67" t="s">
+        <v>797</v>
+      </c>
+      <c r="GT67" t="s">
+        <v>793</v>
+      </c>
+      <c r="GU67" t="s">
+        <v>794</v>
+      </c>
+      <c r="GV67" t="s">
+        <v>795</v>
+      </c>
+      <c r="GW67" t="s">
+        <v>796</v>
+      </c>
+      <c r="GX67" t="s">
+        <v>797</v>
+      </c>
+      <c r="GY67" t="s">
+        <v>793</v>
+      </c>
+      <c r="GZ67" t="s">
+        <v>794</v>
+      </c>
+      <c r="HA67" t="s">
+        <v>795</v>
+      </c>
+      <c r="HB67" t="s">
+        <v>796</v>
+      </c>
+      <c r="HC67" t="s">
+        <v>797</v>
+      </c>
+      <c r="HD67" t="s">
+        <v>793</v>
+      </c>
+      <c r="HE67" t="s">
+        <v>794</v>
+      </c>
+      <c r="HF67" t="s">
+        <v>795</v>
+      </c>
+      <c r="HG67" t="s">
+        <v>796</v>
+      </c>
+      <c r="HH67" t="s">
+        <v>797</v>
+      </c>
+      <c r="HI67" t="s">
+        <v>793</v>
+      </c>
+      <c r="HJ67" t="s">
+        <v>794</v>
+      </c>
+      <c r="HK67" t="s">
+        <v>795</v>
+      </c>
+      <c r="HL67" t="s">
+        <v>796</v>
+      </c>
+      <c r="HM67" t="s">
+        <v>797</v>
+      </c>
+      <c r="HN67" t="s">
+        <v>793</v>
+      </c>
+      <c r="HO67" t="s">
+        <v>794</v>
+      </c>
+      <c r="HP67" t="s">
+        <v>795</v>
+      </c>
+      <c r="HQ67" t="s">
+        <v>796</v>
+      </c>
+      <c r="HR67" t="s">
+        <v>797</v>
+      </c>
+      <c r="HS67" t="s">
+        <v>793</v>
+      </c>
+      <c r="HT67" t="s">
+        <v>794</v>
+      </c>
+      <c r="HU67" t="s">
+        <v>795</v>
+      </c>
+      <c r="HV67" t="s">
+        <v>796</v>
+      </c>
+      <c r="HW67" t="s">
+        <v>797</v>
+      </c>
+      <c r="HX67" t="s">
+        <v>793</v>
+      </c>
+      <c r="HY67" t="s">
+        <v>794</v>
+      </c>
+      <c r="HZ67" t="s">
+        <v>795</v>
+      </c>
+      <c r="IA67" t="s">
+        <v>796</v>
+      </c>
+      <c r="IB67" t="s">
+        <v>797</v>
+      </c>
+      <c r="IC67" t="s">
+        <v>793</v>
+      </c>
+      <c r="ID67" t="s">
+        <v>794</v>
+      </c>
+      <c r="IE67" t="s">
+        <v>795</v>
+      </c>
+      <c r="IF67" t="s">
+        <v>796</v>
+      </c>
+      <c r="IG67" t="s">
+        <v>797</v>
+      </c>
+      <c r="IH67" t="s">
+        <v>793</v>
+      </c>
+      <c r="II67" t="s">
+        <v>794</v>
+      </c>
+      <c r="IJ67" t="s">
+        <v>795</v>
+      </c>
+      <c r="IK67" t="s">
+        <v>796</v>
+      </c>
+      <c r="IL67" t="s">
+        <v>797</v>
+      </c>
+      <c r="IM67" t="s">
+        <v>793</v>
+      </c>
+      <c r="IN67" t="s">
+        <v>794</v>
+      </c>
+      <c r="IO67" t="s">
+        <v>795</v>
+      </c>
+      <c r="IP67" t="s">
+        <v>796</v>
+      </c>
+      <c r="IQ67" t="s">
+        <v>797</v>
+      </c>
+      <c r="IR67" t="s">
+        <v>793</v>
+      </c>
+      <c r="IS67" t="s">
+        <v>794</v>
+      </c>
+      <c r="IT67" t="s">
+        <v>795</v>
+      </c>
+      <c r="IU67" t="s">
+        <v>796</v>
+      </c>
+      <c r="IV67" t="s">
+        <v>797</v>
+      </c>
+      <c r="IW67" t="s">
+        <v>793</v>
+      </c>
+      <c r="IX67" t="s">
+        <v>794</v>
+      </c>
+      <c r="IY67" t="s">
+        <v>795</v>
+      </c>
+      <c r="IZ67" t="s">
+        <v>796</v>
+      </c>
+      <c r="JA67" t="s">
+        <v>797</v>
+      </c>
+      <c r="JB67" t="s">
+        <v>793</v>
+      </c>
+      <c r="JC67" t="s">
+        <v>794</v>
+      </c>
+      <c r="JD67" t="s">
+        <v>795</v>
+      </c>
+      <c r="JE67" t="s">
+        <v>796</v>
+      </c>
+      <c r="JF67" t="s">
+        <v>797</v>
+      </c>
+      <c r="JG67" t="s">
+        <v>793</v>
+      </c>
+      <c r="JH67" t="s">
+        <v>794</v>
+      </c>
+      <c r="JI67" t="s">
+        <v>795</v>
+      </c>
+      <c r="JJ67" t="s">
+        <v>796</v>
+      </c>
+      <c r="JK67" t="s">
+        <v>797</v>
+      </c>
+      <c r="JL67" t="s">
+        <v>793</v>
+      </c>
+      <c r="JM67" t="s">
+        <v>794</v>
+      </c>
+      <c r="JN67" t="s">
+        <v>795</v>
+      </c>
+      <c r="JO67" t="s">
+        <v>796</v>
+      </c>
+      <c r="JP67" t="s">
+        <v>797</v>
+      </c>
+      <c r="JQ67" t="s">
+        <v>793</v>
+      </c>
+      <c r="JR67" t="s">
+        <v>794</v>
+      </c>
+      <c r="JS67" t="s">
+        <v>795</v>
+      </c>
+      <c r="JT67" t="s">
+        <v>796</v>
+      </c>
+      <c r="JU67" t="s">
+        <v>797</v>
+      </c>
+      <c r="JV67" t="s">
+        <v>793</v>
+      </c>
+      <c r="JW67" t="s">
+        <v>794</v>
+      </c>
+      <c r="JX67" t="s">
+        <v>795</v>
+      </c>
+      <c r="JY67" t="s">
+        <v>796</v>
+      </c>
+      <c r="JZ67" t="s">
+        <v>797</v>
+      </c>
+      <c r="KA67" t="s">
+        <v>793</v>
+      </c>
+      <c r="KB67" t="s">
+        <v>794</v>
+      </c>
+      <c r="KC67" t="s">
+        <v>795</v>
+      </c>
+      <c r="KD67" t="s">
+        <v>796</v>
+      </c>
+      <c r="KE67" t="s">
+        <v>797</v>
+      </c>
+      <c r="KF67" t="s">
+        <v>793</v>
+      </c>
+      <c r="KG67" t="s">
+        <v>794</v>
+      </c>
+      <c r="KH67" t="s">
+        <v>795</v>
+      </c>
+      <c r="KI67" t="s">
+        <v>796</v>
+      </c>
+      <c r="KJ67" t="s">
+        <v>797</v>
+      </c>
+      <c r="KK67" t="s">
+        <v>793</v>
+      </c>
+      <c r="KL67" t="s">
+        <v>794</v>
+      </c>
+      <c r="KM67" t="s">
+        <v>795</v>
+      </c>
+      <c r="KN67" t="s">
+        <v>796</v>
+      </c>
+      <c r="KO67" t="s">
+        <v>797</v>
+      </c>
+      <c r="KP67" t="s">
+        <v>793</v>
+      </c>
+      <c r="KQ67" t="s">
+        <v>794</v>
+      </c>
+      <c r="KR67" t="s">
+        <v>795</v>
+      </c>
+      <c r="KS67" t="s">
+        <v>796</v>
+      </c>
+      <c r="KT67" t="s">
+        <v>797</v>
+      </c>
+      <c r="KU67" t="s">
+        <v>793</v>
+      </c>
+      <c r="KV67" t="s">
+        <v>794</v>
+      </c>
+      <c r="KW67" t="s">
+        <v>795</v>
+      </c>
+      <c r="KX67" t="s">
+        <v>796</v>
+      </c>
+      <c r="KY67" t="s">
+        <v>797</v>
+      </c>
+      <c r="KZ67" t="s">
+        <v>793</v>
+      </c>
+      <c r="LA67" t="s">
+        <v>794</v>
+      </c>
+      <c r="LB67" t="s">
+        <v>795</v>
+      </c>
+      <c r="LC67" t="s">
+        <v>796</v>
+      </c>
+      <c r="LD67" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="68" spans="1:316" x14ac:dyDescent="0.3">
@@ -48856,7 +48872,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49226,7 +49242,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>793</v>
+        <v>798</v>
       </c>
       <c r="B10">
         <v>2022</v>
@@ -49276,7 +49292,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>794</v>
+        <v>799</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -49328,50 +49344,50 @@
       <c r="A12" t="s">
         <v>792</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <v>5</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>2</v>
-      </c>
-      <c r="I12">
-        <v>3</v>
-      </c>
-      <c r="J12">
-        <v>4</v>
-      </c>
-      <c r="K12">
-        <v>5</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>2</v>
-      </c>
-      <c r="N12">
-        <v>3</v>
-      </c>
-      <c r="O12">
-        <v>4</v>
-      </c>
-      <c r="P12">
-        <v>5</v>
+      <c r="B12" t="s">
+        <v>793</v>
+      </c>
+      <c r="C12" t="s">
+        <v>794</v>
+      </c>
+      <c r="D12" t="s">
+        <v>795</v>
+      </c>
+      <c r="E12" t="s">
+        <v>796</v>
+      </c>
+      <c r="F12" t="s">
+        <v>797</v>
+      </c>
+      <c r="G12" t="s">
+        <v>793</v>
+      </c>
+      <c r="H12" t="s">
+        <v>794</v>
+      </c>
+      <c r="I12" t="s">
+        <v>795</v>
+      </c>
+      <c r="J12" t="s">
+        <v>796</v>
+      </c>
+      <c r="K12" t="s">
+        <v>797</v>
+      </c>
+      <c r="L12" t="s">
+        <v>793</v>
+      </c>
+      <c r="M12" t="s">
+        <v>794</v>
+      </c>
+      <c r="N12" t="s">
+        <v>795</v>
+      </c>
+      <c r="O12" t="s">
+        <v>796</v>
+      </c>
+      <c r="P12" t="s">
+        <v>797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de la lista taxonómica
Añadí los niveles taxonómicos de Clase, Orden y Familia a la base de datos de fitoplancton.
</commit_message>
<xml_diff>
--- a/datos/crudos/Cajititlán_Bio.xlsx
+++ b/datos/crudos/Cajititlán_Bio.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccopi\Desktop\PP\Caji\datos\crudos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccopi\Desktop\PP\CADO\datos\crudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6B9D36-24FE-442E-8119-3E6284E212F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C319DB90-4BA6-4A53-A9D4-F288AD17CA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{23288B8C-CFF6-477E-BC6E-3C842449D796}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{23288B8C-CFF6-477E-BC6E-3C842449D796}"/>
   </bookViews>
   <sheets>
     <sheet name="Fito" sheetId="4" r:id="rId1"/>
     <sheet name="FitoP" sheetId="5" r:id="rId2"/>
-    <sheet name="Zoo" sheetId="7" r:id="rId3"/>
-    <sheet name="ZooP" sheetId="6" r:id="rId4"/>
-    <sheet name="Junk" sheetId="3" state="hidden" r:id="rId5"/>
+    <sheet name="FitoT" sheetId="8" r:id="rId3"/>
+    <sheet name="Zoo" sheetId="7" r:id="rId4"/>
+    <sheet name="ZooP" sheetId="6" r:id="rId5"/>
+    <sheet name="Junk" sheetId="3" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2198" uniqueCount="887">
   <si>
     <t>Estación</t>
   </si>
@@ -2438,6 +2439,267 @@
   </si>
   <si>
     <t>mes</t>
+  </si>
+  <si>
+    <t>Clase</t>
+  </si>
+  <si>
+    <t>Género</t>
+  </si>
+  <si>
+    <t>Familia</t>
+  </si>
+  <si>
+    <t>Actinastrum</t>
+  </si>
+  <si>
+    <t>Crucigenia</t>
+  </si>
+  <si>
+    <t>Gomphosphaeria</t>
+  </si>
+  <si>
+    <t>Fragilaria</t>
+  </si>
+  <si>
+    <t>Lyngbya</t>
+  </si>
+  <si>
+    <t>Microcystis</t>
+  </si>
+  <si>
+    <t>Scenedesmus</t>
+  </si>
+  <si>
+    <t>Trebouxiophyceae</t>
+  </si>
+  <si>
+    <t>Cyanobacteriia</t>
+  </si>
+  <si>
+    <t>Chlorellales</t>
+  </si>
+  <si>
+    <t>Chlorellaceae</t>
+  </si>
+  <si>
+    <t>Cyanobacteriales</t>
+  </si>
+  <si>
+    <t>Selenastraceae</t>
+  </si>
+  <si>
+    <t>Sphaeropleales</t>
+  </si>
+  <si>
+    <t>Chlorophyceae</t>
+  </si>
+  <si>
+    <t>Nostocaceae</t>
+  </si>
+  <si>
+    <t>Merismopediaceae</t>
+  </si>
+  <si>
+    <t>Microcoleaceae</t>
+  </si>
+  <si>
+    <t>Aulacoseiraceae</t>
+  </si>
+  <si>
+    <t>Euglenaceae</t>
+  </si>
+  <si>
+    <t>Gomphosphaeriaceae</t>
+  </si>
+  <si>
+    <t>Aulacoseirales</t>
+  </si>
+  <si>
+    <t>Bacillariophyceae</t>
+  </si>
+  <si>
+    <t>Botryococcaceae</t>
+  </si>
+  <si>
+    <t>Ceratiaceae</t>
+  </si>
+  <si>
+    <t>Trebouxiales</t>
+  </si>
+  <si>
+    <t>Gonyaulacales</t>
+  </si>
+  <si>
+    <t>Dinophyceae</t>
+  </si>
+  <si>
+    <t>Stephanodicaceae</t>
+  </si>
+  <si>
+    <t>Thalassiosirales</t>
+  </si>
+  <si>
+    <t>Cylindrospermopsis</t>
+  </si>
+  <si>
+    <t>Cylindrospermun</t>
+  </si>
+  <si>
+    <t>Cymbella</t>
+  </si>
+  <si>
+    <t>Cymbellaceae</t>
+  </si>
+  <si>
+    <t>Cymbellales</t>
+  </si>
+  <si>
+    <t>Closteriaceae</t>
+  </si>
+  <si>
+    <t>Zygnematales</t>
+  </si>
+  <si>
+    <t>Zygnematophyceae</t>
+  </si>
+  <si>
+    <t>Scenedesmaceae</t>
+  </si>
+  <si>
+    <t>Microcystaceae</t>
+  </si>
+  <si>
+    <t>Coscinosicaceae</t>
+  </si>
+  <si>
+    <t>Coscinodiscales</t>
+  </si>
+  <si>
+    <t>incertae sedis</t>
+  </si>
+  <si>
+    <t>Volvocaceae</t>
+  </si>
+  <si>
+    <t>Volvocales</t>
+  </si>
+  <si>
+    <t>Euglenida</t>
+  </si>
+  <si>
+    <t>Euglenoidea</t>
+  </si>
+  <si>
+    <t>Gloeocapsa</t>
+  </si>
+  <si>
+    <t>Gloeocapsaceae</t>
+  </si>
+  <si>
+    <t>Fragilariaceae</t>
+  </si>
+  <si>
+    <t>Leptolyngbyaceae</t>
+  </si>
+  <si>
+    <t>Neochloridaceae</t>
+  </si>
+  <si>
+    <t>Naviculaceae</t>
+  </si>
+  <si>
+    <t>Oscillatoriaceae</t>
+  </si>
+  <si>
+    <t>Fragilariales</t>
+  </si>
+  <si>
+    <t>Leptolyngbyales</t>
+  </si>
+  <si>
+    <t>Naviculales</t>
+  </si>
+  <si>
+    <t>Kirchneriella</t>
+  </si>
+  <si>
+    <t>Lepocinclis</t>
+  </si>
+  <si>
+    <t>Phacidae</t>
+  </si>
+  <si>
+    <t>Chamaesiphonaceae</t>
+  </si>
+  <si>
+    <t>Monoraphidium</t>
+  </si>
+  <si>
+    <t>Monoraphidium tortilé</t>
+  </si>
+  <si>
+    <t>Monoraphidium griffithi</t>
+  </si>
+  <si>
+    <t>Surirellaceae</t>
+  </si>
+  <si>
+    <t>Treubariaceae</t>
+  </si>
+  <si>
+    <t>Surirellales</t>
+  </si>
+  <si>
+    <t>Nitzschia</t>
+  </si>
+  <si>
+    <t>Bacillariaceae</t>
+  </si>
+  <si>
+    <t>Bacillariales</t>
+  </si>
+  <si>
+    <t>Oocystaceae</t>
+  </si>
+  <si>
+    <t>Oocystales</t>
+  </si>
+  <si>
+    <t>Planktothrix</t>
+  </si>
+  <si>
+    <t>Planktolyngbya</t>
+  </si>
+  <si>
+    <t>Planktolyngbya sp</t>
+  </si>
+  <si>
+    <t>Pseudanabaena</t>
+  </si>
+  <si>
+    <t>Pseudanabaenaceae</t>
+  </si>
+  <si>
+    <t>Pseudanabaenales</t>
+  </si>
+  <si>
+    <t>Desmidiaceae</t>
+  </si>
+  <si>
+    <t>Synechococcus</t>
+  </si>
+  <si>
+    <t>Synechococcaceae</t>
+  </si>
+  <si>
+    <t>Synechococcales</t>
+  </si>
+  <si>
+    <t>Chlamydomonadales</t>
+  </si>
+  <si>
+    <t>Ochrophyta</t>
   </si>
 </sst>
 </file>
@@ -3100,7 +3362,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3110,7 +3372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F1F480-4040-4F5F-AC98-1E4CE20790A9}">
   <dimension ref="A1:LD65"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
@@ -26626,10 +26888,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD579EC3-DFCC-45CB-8CDA-ACC6EEAB4522}">
-  <dimension ref="A1:LG68"/>
+  <dimension ref="A1:LF68"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67:F67"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="LH4" sqref="LH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26666,15 +26928,20 @@
     <col min="122" max="126" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="127" max="131" width="10" bestFit="1" customWidth="1"/>
     <col min="132" max="136" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="319" max="319" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="318" max="318" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="319" max="319" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="320" max="320" width="18.88671875" customWidth="1"/>
+    <col min="321" max="321" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="322" max="322" width="17" bestFit="1" customWidth="1"/>
+    <col min="323" max="323" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="2" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:318" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>477</v>
       </c>
@@ -27623,11 +27890,8 @@
       <c r="LF2" t="s">
         <v>442</v>
       </c>
-      <c r="LG2" t="s">
-        <v>394</v>
-      </c>
     </row>
-    <row r="3" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>331</v>
       </c>
@@ -28078,11 +28342,8 @@
       <c r="LF3">
         <v>0</v>
       </c>
-      <c r="LG3" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="4" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>332</v>
       </c>
@@ -28105,11 +28366,8 @@
       <c r="LF4">
         <v>1</v>
       </c>
-      <c r="LG4" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="5" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>333</v>
       </c>
@@ -28749,11 +29007,8 @@
       <c r="LF5">
         <v>0</v>
       </c>
-      <c r="LG5" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="6" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>334</v>
       </c>
@@ -28998,11 +29253,8 @@
       <c r="LF6">
         <v>0</v>
       </c>
-      <c r="LG6" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="7" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>335</v>
       </c>
@@ -29187,11 +29439,8 @@
       <c r="LF7">
         <v>1</v>
       </c>
-      <c r="LG7" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="8" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>336</v>
       </c>
@@ -29352,11 +29601,8 @@
       <c r="LF8">
         <v>1</v>
       </c>
-      <c r="LG8" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="9" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>337</v>
       </c>
@@ -29373,11 +29619,8 @@
       <c r="LF9">
         <v>0</v>
       </c>
-      <c r="LG9" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="10" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>338</v>
       </c>
@@ -29684,11 +29927,8 @@
       <c r="LF10">
         <v>0</v>
       </c>
-      <c r="LG10" t="s">
-        <v>397</v>
-      </c>
     </row>
-    <row r="11" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>339</v>
       </c>
@@ -29792,11 +30032,8 @@
       <c r="LF11">
         <v>0</v>
       </c>
-      <c r="LG11" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="12" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>340</v>
       </c>
@@ -29807,11 +30044,8 @@
       <c r="LF12">
         <v>0</v>
       </c>
-      <c r="LG12" t="s">
-        <v>398</v>
-      </c>
     </row>
-    <row r="13" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>399</v>
       </c>
@@ -30035,13 +30269,10 @@
       <c r="LF13">
         <v>0</v>
       </c>
-      <c r="LG13" t="s">
-        <v>397</v>
-      </c>
     </row>
-    <row r="14" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>342</v>
+        <v>833</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -30970,13 +31201,10 @@
       <c r="LF14">
         <v>1</v>
       </c>
-      <c r="LG14" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="15" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>343</v>
+        <v>834</v>
       </c>
       <c r="V15" s="23"/>
       <c r="CY15">
@@ -31156,13 +31384,10 @@
       <c r="LF15">
         <v>1</v>
       </c>
-      <c r="LG15" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="16" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>344</v>
+        <v>835</v>
       </c>
       <c r="I16">
         <v>3</v>
@@ -31219,11 +31444,8 @@
       <c r="LF16">
         <v>0</v>
       </c>
-      <c r="LG16" t="s">
-        <v>397</v>
-      </c>
     </row>
-    <row r="17" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>345</v>
       </c>
@@ -31977,11 +32199,8 @@
       <c r="LF17">
         <v>0</v>
       </c>
-      <c r="LG17" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="18" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>346</v>
       </c>
@@ -32091,11 +32310,8 @@
       <c r="LF18">
         <v>0</v>
       </c>
-      <c r="LG18" t="s">
-        <v>400</v>
-      </c>
     </row>
-    <row r="19" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>347</v>
       </c>
@@ -32403,11 +32619,8 @@
       <c r="LF19">
         <v>0</v>
       </c>
-      <c r="LG19" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="20" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>348</v>
       </c>
@@ -32442,11 +32655,8 @@
       <c r="LF20">
         <v>0</v>
       </c>
-      <c r="LG20" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="21" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>349</v>
       </c>
@@ -32582,11 +32792,8 @@
       <c r="LF21">
         <v>0</v>
       </c>
-      <c r="LG21" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="22" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>350</v>
       </c>
@@ -32654,11 +32861,8 @@
       <c r="LF22">
         <v>0</v>
       </c>
-      <c r="LG22" t="s">
-        <v>397</v>
-      </c>
     </row>
-    <row r="23" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>351</v>
       </c>
@@ -32935,11 +33139,8 @@
       <c r="LF23">
         <v>0</v>
       </c>
-      <c r="LG23" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="24" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>352</v>
       </c>
@@ -32995,11 +33196,8 @@
       <c r="LF24">
         <v>0</v>
       </c>
-      <c r="LG24" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="25" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>401</v>
       </c>
@@ -33094,11 +33292,8 @@
       <c r="LF25">
         <v>0</v>
       </c>
-      <c r="LG25" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="26" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>354</v>
       </c>
@@ -33651,11 +33846,8 @@
       <c r="LF26">
         <v>0</v>
       </c>
-      <c r="LG26" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="27" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>355</v>
       </c>
@@ -33959,13 +34151,10 @@
       <c r="LF27">
         <v>0</v>
       </c>
-      <c r="LG27" t="s">
-        <v>402</v>
-      </c>
     </row>
-    <row r="28" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>356</v>
+        <v>850</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -34231,11 +34420,8 @@
       <c r="LF28">
         <v>0</v>
       </c>
-      <c r="LG28" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="29" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>357</v>
       </c>
@@ -34345,11 +34531,8 @@
       <c r="LF29">
         <v>0</v>
       </c>
-      <c r="LG29" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="30" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>358</v>
       </c>
@@ -34405,11 +34588,8 @@
       <c r="LF30">
         <v>0</v>
       </c>
-      <c r="LG30" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="31" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>359</v>
       </c>
@@ -34585,13 +34765,10 @@
       <c r="LF31">
         <v>0</v>
       </c>
-      <c r="LG31" t="s">
-        <v>397</v>
-      </c>
     </row>
-    <row r="32" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>360</v>
+        <v>860</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -35122,11 +35299,8 @@
       <c r="LF32">
         <v>0</v>
       </c>
-      <c r="LG32" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="33" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>361</v>
       </c>
@@ -35388,13 +35562,10 @@
       <c r="LF33">
         <v>0</v>
       </c>
-      <c r="LG33" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="34" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>362</v>
+        <v>861</v>
       </c>
       <c r="V34" s="23"/>
       <c r="CK34">
@@ -35451,11 +35622,8 @@
       <c r="LF34">
         <v>0</v>
       </c>
-      <c r="LG34" t="s">
-        <v>402</v>
-      </c>
     </row>
-    <row r="35" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>363</v>
       </c>
@@ -35568,11 +35736,8 @@
       <c r="LF35">
         <v>1</v>
       </c>
-      <c r="LG35" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="36" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>364</v>
       </c>
@@ -36416,11 +36581,8 @@
       <c r="LF36">
         <v>0</v>
       </c>
-      <c r="LG36" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="37" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>365</v>
       </c>
@@ -36434,11 +36596,8 @@
       <c r="LF37">
         <v>0</v>
       </c>
-      <c r="LG37" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="38" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>403</v>
       </c>
@@ -36940,13 +37099,10 @@
       <c r="LF38">
         <v>1</v>
       </c>
-      <c r="LG38" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="39" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>367</v>
+        <v>865</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -37386,13 +37542,10 @@
       <c r="LF39">
         <v>0</v>
       </c>
-      <c r="LG39" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="40" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>368</v>
+        <v>866</v>
       </c>
       <c r="V40" s="23"/>
       <c r="AF40">
@@ -37683,11 +37836,8 @@
       <c r="LF40">
         <v>0</v>
       </c>
-      <c r="LG40" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="41" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>369</v>
       </c>
@@ -38018,13 +38168,10 @@
       <c r="LF41">
         <v>0</v>
       </c>
-      <c r="LG41" t="s">
-        <v>397</v>
-      </c>
     </row>
-    <row r="42" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>370</v>
+        <v>870</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -38255,11 +38402,8 @@
       <c r="LF42">
         <v>0</v>
       </c>
-      <c r="LG42" t="s">
-        <v>397</v>
-      </c>
     </row>
-    <row r="43" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>371</v>
       </c>
@@ -38801,11 +38945,8 @@
       <c r="LF43">
         <v>1</v>
       </c>
-      <c r="LG43" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="44" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>372</v>
       </c>
@@ -39086,11 +39227,8 @@
       <c r="LF44">
         <v>0</v>
       </c>
-      <c r="LG44" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="45" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>374</v>
       </c>
@@ -39224,11 +39362,8 @@
       <c r="LF45">
         <v>0</v>
       </c>
-      <c r="LG45" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="46" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>375</v>
       </c>
@@ -39643,13 +39778,10 @@
       <c r="LF46">
         <v>0</v>
       </c>
-      <c r="LG46" t="s">
-        <v>402</v>
-      </c>
     </row>
-    <row r="47" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>376</v>
+        <v>875</v>
       </c>
       <c r="B47">
         <v>13</v>
@@ -40302,13 +40434,10 @@
       <c r="LF47">
         <v>1</v>
       </c>
-      <c r="LG47" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="48" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>377</v>
+        <v>877</v>
       </c>
       <c r="B48">
         <v>25</v>
@@ -40568,13 +40697,10 @@
       <c r="LF48">
         <v>1</v>
       </c>
-      <c r="LG48" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="49" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>378</v>
+        <v>878</v>
       </c>
       <c r="V49" s="23"/>
       <c r="AF49">
@@ -40778,11 +40904,8 @@
       <c r="LF49">
         <v>1</v>
       </c>
-      <c r="LG49" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="50" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>379</v>
       </c>
@@ -41674,11 +41797,8 @@
       <c r="LF50">
         <v>1</v>
       </c>
-      <c r="LG50" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="51" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>380</v>
       </c>
@@ -41838,11 +41958,8 @@
       <c r="LF51">
         <v>1</v>
       </c>
-      <c r="LG51" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="52" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>381</v>
       </c>
@@ -42566,11 +42683,8 @@
       <c r="LF52">
         <v>0</v>
       </c>
-      <c r="LG52" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="53" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>382</v>
       </c>
@@ -42745,11 +42859,8 @@
       <c r="LF53">
         <v>0</v>
       </c>
-      <c r="LG53" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="54" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>383</v>
       </c>
@@ -43132,11 +43243,8 @@
       <c r="LF54">
         <v>0</v>
       </c>
-      <c r="LG54" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="55" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>384</v>
       </c>
@@ -43548,11 +43656,8 @@
       <c r="LF55">
         <v>0</v>
       </c>
-      <c r="LG55" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="56" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>385</v>
       </c>
@@ -43596,11 +43701,8 @@
       <c r="LF56">
         <v>1</v>
       </c>
-      <c r="LG56" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="57" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>386</v>
       </c>
@@ -43632,11 +43734,8 @@
       <c r="LF57">
         <v>0</v>
       </c>
-      <c r="LG57" t="s">
-        <v>397</v>
-      </c>
     </row>
-    <row r="58" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>387</v>
       </c>
@@ -43650,11 +43749,8 @@
       <c r="LF58">
         <v>0</v>
       </c>
-      <c r="LG58" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="59" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>388</v>
       </c>
@@ -43944,11 +44040,8 @@
       <c r="LF59">
         <v>0</v>
       </c>
-      <c r="LG59" t="s">
-        <v>397</v>
-      </c>
     </row>
-    <row r="60" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>390</v>
       </c>
@@ -44295,11 +44388,8 @@
       <c r="LF60">
         <v>1</v>
       </c>
-      <c r="LG60" t="s">
-        <v>396</v>
-      </c>
     </row>
-    <row r="61" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>391</v>
       </c>
@@ -44376,11 +44466,8 @@
       <c r="LF61">
         <v>0</v>
       </c>
-      <c r="LG61" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="62" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>392</v>
       </c>
@@ -44541,11 +44628,8 @@
       <c r="LF62">
         <v>0</v>
       </c>
-      <c r="LG62" t="s">
-        <v>395</v>
-      </c>
     </row>
-    <row r="63" spans="1:319" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:318" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>393</v>
       </c>
@@ -44651,9 +44735,6 @@
       </c>
       <c r="LF63">
         <v>1</v>
-      </c>
-      <c r="LG63" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="65" spans="1:316" x14ac:dyDescent="0.3">
@@ -48462,6 +48543,1000 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDA0173-877B-40F6-8E72-B4008AD4C354}">
+  <dimension ref="A1:E57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1" t="s">
+        <v>800</v>
+      </c>
+      <c r="C1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1" t="s">
+        <v>802</v>
+      </c>
+      <c r="E1" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B2" t="s">
+        <v>825</v>
+      </c>
+      <c r="C2" t="s">
+        <v>824</v>
+      </c>
+      <c r="D2" t="s">
+        <v>821</v>
+      </c>
+      <c r="E2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B3" t="s">
+        <v>825</v>
+      </c>
+      <c r="C3" t="s">
+        <v>837</v>
+      </c>
+      <c r="D3" t="s">
+        <v>836</v>
+      </c>
+      <c r="E3" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>397</v>
+      </c>
+      <c r="B4" t="s">
+        <v>825</v>
+      </c>
+      <c r="C4" t="s">
+        <v>844</v>
+      </c>
+      <c r="D4" t="s">
+        <v>843</v>
+      </c>
+      <c r="E4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>397</v>
+      </c>
+      <c r="B5" t="s">
+        <v>825</v>
+      </c>
+      <c r="C5" t="s">
+        <v>857</v>
+      </c>
+      <c r="D5" t="s">
+        <v>852</v>
+      </c>
+      <c r="E5" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>397</v>
+      </c>
+      <c r="B6" t="s">
+        <v>825</v>
+      </c>
+      <c r="C6" t="s">
+        <v>859</v>
+      </c>
+      <c r="D6" t="s">
+        <v>855</v>
+      </c>
+      <c r="E6" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>397</v>
+      </c>
+      <c r="B7" t="s">
+        <v>825</v>
+      </c>
+      <c r="C7" t="s">
+        <v>872</v>
+      </c>
+      <c r="D7" t="s">
+        <v>871</v>
+      </c>
+      <c r="E7" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>397</v>
+      </c>
+      <c r="B8" t="s">
+        <v>825</v>
+      </c>
+      <c r="C8" t="s">
+        <v>869</v>
+      </c>
+      <c r="D8" t="s">
+        <v>867</v>
+      </c>
+      <c r="E8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>400</v>
+      </c>
+      <c r="B9" t="s">
+        <v>840</v>
+      </c>
+      <c r="C9" t="s">
+        <v>839</v>
+      </c>
+      <c r="D9" t="s">
+        <v>838</v>
+      </c>
+      <c r="E9" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>400</v>
+      </c>
+      <c r="B10" t="s">
+        <v>840</v>
+      </c>
+      <c r="C10" t="s">
+        <v>839</v>
+      </c>
+      <c r="D10" t="s">
+        <v>881</v>
+      </c>
+      <c r="E10" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>395</v>
+      </c>
+      <c r="B11" t="s">
+        <v>810</v>
+      </c>
+      <c r="C11" t="s">
+        <v>812</v>
+      </c>
+      <c r="D11" t="s">
+        <v>813</v>
+      </c>
+      <c r="E11" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>395</v>
+      </c>
+      <c r="B12" t="s">
+        <v>817</v>
+      </c>
+      <c r="C12" t="s">
+        <v>885</v>
+      </c>
+      <c r="D12" t="s">
+        <v>868</v>
+      </c>
+      <c r="E12" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>395</v>
+      </c>
+      <c r="B13" t="s">
+        <v>817</v>
+      </c>
+      <c r="C13" t="s">
+        <v>812</v>
+      </c>
+      <c r="D13" t="s">
+        <v>813</v>
+      </c>
+      <c r="E13" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>395</v>
+      </c>
+      <c r="B14" t="s">
+        <v>817</v>
+      </c>
+      <c r="C14" t="s">
+        <v>816</v>
+      </c>
+      <c r="D14" t="s">
+        <v>854</v>
+      </c>
+      <c r="E14" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>395</v>
+      </c>
+      <c r="B15" t="s">
+        <v>817</v>
+      </c>
+      <c r="C15" t="s">
+        <v>816</v>
+      </c>
+      <c r="D15" t="s">
+        <v>841</v>
+      </c>
+      <c r="E15" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>395</v>
+      </c>
+      <c r="B16" t="s">
+        <v>817</v>
+      </c>
+      <c r="C16" t="s">
+        <v>816</v>
+      </c>
+      <c r="D16" t="s">
+        <v>841</v>
+      </c>
+      <c r="E16" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>395</v>
+      </c>
+      <c r="B17" t="s">
+        <v>817</v>
+      </c>
+      <c r="C17" t="s">
+        <v>816</v>
+      </c>
+      <c r="D17" t="s">
+        <v>841</v>
+      </c>
+      <c r="E17" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>395</v>
+      </c>
+      <c r="B18" t="s">
+        <v>817</v>
+      </c>
+      <c r="C18" t="s">
+        <v>816</v>
+      </c>
+      <c r="D18" t="s">
+        <v>815</v>
+      </c>
+      <c r="E18" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>395</v>
+      </c>
+      <c r="B19" t="s">
+        <v>817</v>
+      </c>
+      <c r="C19" t="s">
+        <v>816</v>
+      </c>
+      <c r="D19" t="s">
+        <v>815</v>
+      </c>
+      <c r="E19" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>395</v>
+      </c>
+      <c r="B20" t="s">
+        <v>817</v>
+      </c>
+      <c r="C20" t="s">
+        <v>816</v>
+      </c>
+      <c r="D20" t="s">
+        <v>815</v>
+      </c>
+      <c r="E20" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>395</v>
+      </c>
+      <c r="B21" t="s">
+        <v>817</v>
+      </c>
+      <c r="C21" t="s">
+        <v>816</v>
+      </c>
+      <c r="D21" t="s">
+        <v>815</v>
+      </c>
+      <c r="E21" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>395</v>
+      </c>
+      <c r="B22" t="s">
+        <v>817</v>
+      </c>
+      <c r="C22" t="s">
+        <v>847</v>
+      </c>
+      <c r="D22" t="s">
+        <v>846</v>
+      </c>
+      <c r="E22" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>395</v>
+      </c>
+      <c r="B23" t="s">
+        <v>817</v>
+      </c>
+      <c r="C23" t="s">
+        <v>847</v>
+      </c>
+      <c r="D23" t="s">
+        <v>846</v>
+      </c>
+      <c r="E23" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>395</v>
+      </c>
+      <c r="B24" t="s">
+        <v>810</v>
+      </c>
+      <c r="C24" t="s">
+        <v>812</v>
+      </c>
+      <c r="D24" t="s">
+        <v>813</v>
+      </c>
+      <c r="E24" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>395</v>
+      </c>
+      <c r="B25" t="s">
+        <v>810</v>
+      </c>
+      <c r="C25" t="s">
+        <v>812</v>
+      </c>
+      <c r="D25" t="s">
+        <v>813</v>
+      </c>
+      <c r="E25" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>395</v>
+      </c>
+      <c r="B26" t="s">
+        <v>810</v>
+      </c>
+      <c r="C26" t="s">
+        <v>845</v>
+      </c>
+      <c r="D26" t="s">
+        <v>845</v>
+      </c>
+      <c r="E26" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>395</v>
+      </c>
+      <c r="B27" t="s">
+        <v>810</v>
+      </c>
+      <c r="C27" t="s">
+        <v>874</v>
+      </c>
+      <c r="D27" t="s">
+        <v>873</v>
+      </c>
+      <c r="E27" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>395</v>
+      </c>
+      <c r="B28" t="s">
+        <v>810</v>
+      </c>
+      <c r="C28" t="s">
+        <v>828</v>
+      </c>
+      <c r="D28" t="s">
+        <v>826</v>
+      </c>
+      <c r="E28" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>396</v>
+      </c>
+      <c r="B29" t="s">
+        <v>811</v>
+      </c>
+      <c r="C29" t="s">
+        <v>814</v>
+      </c>
+      <c r="D29" t="s">
+        <v>863</v>
+      </c>
+      <c r="E29" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>396</v>
+      </c>
+      <c r="B30" t="s">
+        <v>811</v>
+      </c>
+      <c r="C30" t="s">
+        <v>814</v>
+      </c>
+      <c r="D30" t="s">
+        <v>851</v>
+      </c>
+      <c r="E30" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>396</v>
+      </c>
+      <c r="B31" t="s">
+        <v>811</v>
+      </c>
+      <c r="C31" t="s">
+        <v>814</v>
+      </c>
+      <c r="D31" t="s">
+        <v>823</v>
+      </c>
+      <c r="E31" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>396</v>
+      </c>
+      <c r="B32" t="s">
+        <v>811</v>
+      </c>
+      <c r="C32" t="s">
+        <v>814</v>
+      </c>
+      <c r="D32" t="s">
+        <v>823</v>
+      </c>
+      <c r="E32" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>396</v>
+      </c>
+      <c r="B33" t="s">
+        <v>811</v>
+      </c>
+      <c r="C33" t="s">
+        <v>814</v>
+      </c>
+      <c r="D33" t="s">
+        <v>820</v>
+      </c>
+      <c r="E33" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>396</v>
+      </c>
+      <c r="B34" t="s">
+        <v>811</v>
+      </c>
+      <c r="C34" t="s">
+        <v>814</v>
+      </c>
+      <c r="D34" t="s">
+        <v>820</v>
+      </c>
+      <c r="E34" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>396</v>
+      </c>
+      <c r="B35" t="s">
+        <v>811</v>
+      </c>
+      <c r="C35" t="s">
+        <v>814</v>
+      </c>
+      <c r="D35" t="s">
+        <v>820</v>
+      </c>
+      <c r="E35" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>396</v>
+      </c>
+      <c r="B36" t="s">
+        <v>811</v>
+      </c>
+      <c r="C36" t="s">
+        <v>814</v>
+      </c>
+      <c r="D36" t="s">
+        <v>842</v>
+      </c>
+      <c r="E36" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>396</v>
+      </c>
+      <c r="B37" t="s">
+        <v>811</v>
+      </c>
+      <c r="C37" t="s">
+        <v>814</v>
+      </c>
+      <c r="D37" t="s">
+        <v>842</v>
+      </c>
+      <c r="E37" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>396</v>
+      </c>
+      <c r="B38" t="s">
+        <v>811</v>
+      </c>
+      <c r="C38" t="s">
+        <v>814</v>
+      </c>
+      <c r="D38" t="s">
+        <v>842</v>
+      </c>
+      <c r="E38" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>396</v>
+      </c>
+      <c r="B39" t="s">
+        <v>811</v>
+      </c>
+      <c r="C39" t="s">
+        <v>814</v>
+      </c>
+      <c r="D39" t="s">
+        <v>842</v>
+      </c>
+      <c r="E39" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>396</v>
+      </c>
+      <c r="B40" t="s">
+        <v>811</v>
+      </c>
+      <c r="C40" t="s">
+        <v>814</v>
+      </c>
+      <c r="D40" t="s">
+        <v>818</v>
+      </c>
+      <c r="E40" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>396</v>
+      </c>
+      <c r="B41" t="s">
+        <v>811</v>
+      </c>
+      <c r="C41" t="s">
+        <v>814</v>
+      </c>
+      <c r="D41" t="s">
+        <v>818</v>
+      </c>
+      <c r="E41" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>396</v>
+      </c>
+      <c r="B42" t="s">
+        <v>811</v>
+      </c>
+      <c r="C42" t="s">
+        <v>814</v>
+      </c>
+      <c r="D42" t="s">
+        <v>818</v>
+      </c>
+      <c r="E42" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>396</v>
+      </c>
+      <c r="B43" t="s">
+        <v>811</v>
+      </c>
+      <c r="C43" t="s">
+        <v>814</v>
+      </c>
+      <c r="D43" t="s">
+        <v>818</v>
+      </c>
+      <c r="E43" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>396</v>
+      </c>
+      <c r="B44" t="s">
+        <v>811</v>
+      </c>
+      <c r="C44" t="s">
+        <v>814</v>
+      </c>
+      <c r="D44" t="s">
+        <v>818</v>
+      </c>
+      <c r="E44" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>396</v>
+      </c>
+      <c r="B45" t="s">
+        <v>811</v>
+      </c>
+      <c r="C45" t="s">
+        <v>814</v>
+      </c>
+      <c r="D45" t="s">
+        <v>856</v>
+      </c>
+      <c r="E45" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>396</v>
+      </c>
+      <c r="B46" t="s">
+        <v>811</v>
+      </c>
+      <c r="C46" t="s">
+        <v>858</v>
+      </c>
+      <c r="D46" t="s">
+        <v>853</v>
+      </c>
+      <c r="E46" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>396</v>
+      </c>
+      <c r="B47" t="s">
+        <v>811</v>
+      </c>
+      <c r="C47" t="s">
+        <v>858</v>
+      </c>
+      <c r="D47" t="s">
+        <v>853</v>
+      </c>
+      <c r="E47" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>396</v>
+      </c>
+      <c r="B48" t="s">
+        <v>811</v>
+      </c>
+      <c r="C48" t="s">
+        <v>880</v>
+      </c>
+      <c r="D48" t="s">
+        <v>879</v>
+      </c>
+      <c r="E48" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>396</v>
+      </c>
+      <c r="B49" t="s">
+        <v>811</v>
+      </c>
+      <c r="C49" t="s">
+        <v>884</v>
+      </c>
+      <c r="D49" t="s">
+        <v>819</v>
+      </c>
+      <c r="E49" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>396</v>
+      </c>
+      <c r="B50" t="s">
+        <v>811</v>
+      </c>
+      <c r="C50" t="s">
+        <v>884</v>
+      </c>
+      <c r="D50" t="s">
+        <v>819</v>
+      </c>
+      <c r="E50" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>396</v>
+      </c>
+      <c r="B51" t="s">
+        <v>811</v>
+      </c>
+      <c r="C51" t="s">
+        <v>884</v>
+      </c>
+      <c r="D51" t="s">
+        <v>883</v>
+      </c>
+      <c r="E51" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>402</v>
+      </c>
+      <c r="B52" t="s">
+        <v>849</v>
+      </c>
+      <c r="C52" t="s">
+        <v>848</v>
+      </c>
+      <c r="D52" t="s">
+        <v>822</v>
+      </c>
+      <c r="E52" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>402</v>
+      </c>
+      <c r="B53" t="s">
+        <v>849</v>
+      </c>
+      <c r="C53" t="s">
+        <v>848</v>
+      </c>
+      <c r="D53" t="s">
+        <v>862</v>
+      </c>
+      <c r="E53" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>402</v>
+      </c>
+      <c r="B54" t="s">
+        <v>849</v>
+      </c>
+      <c r="C54" t="s">
+        <v>848</v>
+      </c>
+      <c r="D54" t="s">
+        <v>862</v>
+      </c>
+      <c r="E54" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>398</v>
+      </c>
+      <c r="B55" t="s">
+        <v>830</v>
+      </c>
+      <c r="C55" t="s">
+        <v>829</v>
+      </c>
+      <c r="D55" t="s">
+        <v>827</v>
+      </c>
+      <c r="E55" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>886</v>
+      </c>
+      <c r="B56" t="s">
+        <v>825</v>
+      </c>
+      <c r="C56" t="s">
+        <v>832</v>
+      </c>
+      <c r="D56" t="s">
+        <v>831</v>
+      </c>
+      <c r="E56" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>886</v>
+      </c>
+      <c r="B57" t="s">
+        <v>825</v>
+      </c>
+      <c r="C57" t="s">
+        <v>832</v>
+      </c>
+      <c r="D57" t="s">
+        <v>831</v>
+      </c>
+      <c r="E57" t="s">
+        <v>388</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D29:E45">
+    <sortCondition ref="D45"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209B4561-73B3-43BF-AFD3-CD6A00461579}">
   <dimension ref="A1:P8"/>
   <sheetViews>
@@ -48867,11 +49942,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D2850C-6343-47D5-B8B0-A4229DF3B723}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
@@ -49395,7 +50470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08232203-5B4E-46B2-890F-6CA4DDB385AC}">
   <dimension ref="A2:AW287"/>
   <sheetViews>

</xml_diff>